<commit_message>
changement nom script + creation script pour creer NETWORK +
</commit_message>
<xml_diff>
--- a/matrice-template.xlsx
+++ b/matrice-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julien.bossuet\PycharmProjects\stormshield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA2C934F-3E61-47F2-81A2-50662D445637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96597DC8-13EB-460F-B89D-BA1F88906DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE8F6597-7D45-4387-84DE-E65C5C822192}"/>
   </bookViews>
@@ -36,43 +36,175 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
   <si>
     <t xml:space="preserve">                       DESTINATION
 SOURCE</t>
   </si>
   <si>
-    <t>VM1
-172.16.1.0/24</t>
-  </si>
-  <si>
-    <t>VM2
-172.16.2.0/24</t>
-  </si>
-  <si>
-    <t>TCP-25
-TCP-389</t>
-  </si>
-  <si>
-    <t>TCP-443</t>
-  </si>
-  <si>
-    <t>TCP-88</t>
-  </si>
-  <si>
-    <t>UDP-25
-TCP-25
-TCP-3389</t>
+    <t>VM-SRVVCCS-01
+10.10.1.14/24</t>
+  </si>
+  <si>
+    <t>VM-SRVVSPC-01
+10.10.1.13/24</t>
+  </si>
+  <si>
+    <t>VM-SRVVSPCWEB-01
+172.20.1.3/24</t>
+  </si>
+  <si>
+    <t>VM-SRVVCCGW-01
+172.20.1.1/24</t>
+  </si>
+  <si>
+    <t>VM-SRVVCCGW-02
+172.20.1.2/24</t>
+  </si>
+  <si>
+    <t>TCP_135
+TCP_445
+TCP_49152-65535</t>
+  </si>
+  <si>
+    <t>TCP_9999</t>
+  </si>
+  <si>
+    <t>TCP_6160
+TCP_6168
+TCP_2500-3300</t>
+  </si>
+  <si>
+    <t>TCP_6169
+TCP_8190-8191
+TCP_2500-5000
+TCP_6185</t>
+  </si>
+  <si>
+    <t>VM-SRVREPOXFS-01
+10.20.1.1/24</t>
+  </si>
+  <si>
+    <t>(VSPC)</t>
+  </si>
+  <si>
+    <t>VM-SRVVB365S-01
+10.10.1.15</t>
+  </si>
+  <si>
+    <t>VM-SRVVB365PXY-01
+10.20.1.2</t>
+  </si>
+  <si>
+    <t>REPO WIN</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>WAN ACC</t>
+  </si>
+  <si>
+    <t>SRVVOM-01
+10.10.1.16</t>
+  </si>
+  <si>
+    <t>VM-SRVVCSPCDB-01
+10.30.1.1</t>
+  </si>
+  <si>
+    <t>TCP_443</t>
+  </si>
+  <si>
+    <t>TCP_1433</t>
+  </si>
+  <si>
+    <t>TCP_445
+TCP_135
+TCP_6160
+TCP_6162
+TCP_49152-65535
+TCP_2500-3300</t>
+  </si>
+  <si>
+    <t>TCP_22
+TCP_6160
+TCP_6162
+TCP_2500-3300</t>
+  </si>
+  <si>
+    <t>TCP_2500-3300
+TCP_443
+TCP_80</t>
+  </si>
+  <si>
+    <t>TCP_445
+TCP_135
+TCP_6160
+TCP_6162
+TCP_6164
+TCP_6220
+TCP_49152-65535</t>
+  </si>
+  <si>
+    <t>TCP_2500-5000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCP_2500-5000
+</t>
+  </si>
+  <si>
+    <t>TCP_6165</t>
+  </si>
+  <si>
+    <t>TCP_9194</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">VM-SRVVSPC-01
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10.10.1.13/24</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -85,13 +217,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -138,17 +318,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,94 +691,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA8C873-C9D3-465E-A2CF-9C81838AD70F}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="31.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="1" max="16384" width="31.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>